<commit_message>
update intro, minor restructure of body
</commit_message>
<xml_diff>
--- a/figures/PSSI Pillars Overview.xlsx
+++ b/figures/PSSI Pillars Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://086gc-my.sharepoint.com/personal/cory_lagasse_dfo-mpo_gc_ca/Documents/0.Workspace/PSSI-final-tech-report/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="11_F25DC773A252ABDACC1048A781595F1C5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A10988CC-9171-4AE4-9F89-EC087A90FFBC}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="11_F25DC773A252ABDACC1048A781595F1C5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4B39AB1-2055-4126-9AA8-8CFD70B844CA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Pillar</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>Sub-initiative</t>
+  </si>
+  <si>
+    <t>Improved Understanding of Salmon Ecosystems</t>
+  </si>
+  <si>
+    <t>International Science and Monitoring (High Seas Survey)</t>
+  </si>
+  <si>
+    <t>Salmon Habitat Restoration Centre for Expertise</t>
   </si>
 </sst>
 </file>
@@ -299,7 +308,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,169 +695,228 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE26712E-1FD9-4234-986F-6FAB3FE6658B}">
-  <dimension ref="A3:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="11.109375" customWidth="1"/>
     <col min="4" max="4" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>2.1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6">
-        <v>6.1</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>4.2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
       <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="6">
-        <v>7.1</v>
+        <v>6.1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>2</v>
+      </c>
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="6">
-        <v>8.1</v>
+        <v>7.1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>2</v>
+      </c>
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="6">
-        <v>8.1999999999999993</v>
+        <v>8.1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>2</v>
+      </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="6">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6">
         <v>9.1</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="8" t="s">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C10" s="6">
         <v>9.1999999999999993</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="6">
         <v>10.1</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="8" t="s">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C12" s="6">
         <v>10.199999999999999</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="5" t="s">
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C13" s="6">
         <v>10.3</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="8" t="s">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C14" s="6">
         <v>10.4</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="9" t="s">
+    <row r="15" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C15" s="10">
         <v>10.5</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A4:A14"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>